<commit_message>
Primera pasada de correcciones
</commit_message>
<xml_diff>
--- a/Guia03 - Dualidad y Sensibilidad/xls/Tablas.xlsx
+++ b/Guia03 - Dualidad y Sensibilidad/xls/Tablas.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Tabla1" sheetId="1" r:id="rId1"/>
     <sheet name="Excel2LaTeX" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="Tabla2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,13 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
-  <si>
-    <t>Cambios en los parametros</t>
-  </si>
-  <si>
-    <t>Propiedad de la solucion afectada</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="76">
   <si>
     <t>Procedimiento para reoptimizar desde el primal</t>
   </si>
@@ -41,9 +35,6 @@
     <t>Agregado de una nueva Actividad</t>
   </si>
   <si>
-    <t>Agregado de una nueva restriccion</t>
-  </si>
-  <si>
     <t>Problema</t>
   </si>
   <si>
@@ -59,12 +50,6 @@
     <t>D</t>
   </si>
   <si>
-    <t>Optima unica</t>
-  </si>
-  <si>
-    <t>Optima Unica</t>
-  </si>
-  <si>
     <t>No Acotada</t>
   </si>
   <si>
@@ -86,9 +71,6 @@
     <t>FileName</t>
   </si>
   <si>
-    <t xml:space="preserve">Tipo de Solucion </t>
-  </si>
-  <si>
     <t>PRIMAL</t>
   </si>
   <si>
@@ -203,49 +185,70 @@
     <t>Debemos trabajar sobre el problema dual asociado</t>
   </si>
   <si>
-    <t>Debemos recalcular el renglon $\zero$.   En caso de que no sea optimo, seguimos iterando</t>
-  </si>
-  <si>
-    <t>Verificamos si la solucion optima actual verifica la restriccion modificada.  En caso de no hacerlo es necesario modificar la tabla y trabajar sobre el primal asociado</t>
-  </si>
-  <si>
-    <t>Verificamos si la solucion optima cumple con la restriccion modificada.  En caso de que no sea asi modificamos la tabla y trabajamos sobre el problema dual</t>
-  </si>
-  <si>
-    <t>Verificamos si la solucion optima lo sigue siendo (analizando el renglon $\zero$).   Caso contrario re iteramos.</t>
-  </si>
-  <si>
-    <t>Agregamos una nueva columna a la tabla optima.  Verificamos si la solucion optima lo sigue siendo (analizando el renglon $\zero$) y en caso contrario re iteramos.</t>
-  </si>
-  <si>
-    <t>La nueva actividad se convierte en una nueva restrccion.   La reoptimizacion es analoga al caso de nueva nueva restriccion en el primal</t>
-  </si>
-  <si>
-    <t>Verificamos si la solucion optima cumple con la restriccion modificada.   En caso de que no sea asi modificamos la tabla y trabajamos sobre el problema dual</t>
-  </si>
-  <si>
-    <t>La nueva restriccion se convierte en una nueva actividad.    La reoptimizacion es analoga al caso de nueva nueva actividad  en el primal</t>
-  </si>
-  <si>
     <t>Cambio en $a_{ij}$ no basica</t>
   </si>
   <si>
-    <t>Recalulamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.  Verificamos si la solucion optima lo sigue siendo (analizando el renglon $\zero$) y en caso contrario re iteramos.</t>
-  </si>
-  <si>
     <t>Cambio en $a_{ij}$ basica</t>
   </si>
   <si>
-    <t>Recalulamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.   Verificamos si la solucion optima lo sigue siendo (analizando el renglon $\zero$) y en caso contrario re iteramos.</t>
-  </si>
-  <si>
     <t>Correspondencia</t>
   </si>
   <si>
-    <t>Valores Basicos</t>
-  </si>
-  <si>
-    <t>No Basicas</t>
+    <t xml:space="preserve">Tipo de Solución </t>
+  </si>
+  <si>
+    <t>Valores Básicos</t>
+  </si>
+  <si>
+    <t>No Básicas</t>
+  </si>
+  <si>
+    <t>Optima única</t>
+  </si>
+  <si>
+    <t>Optima Única</t>
+  </si>
+  <si>
+    <t>Verificamos si la solución optima actual verifica la restricción modificada.  En caso de no hacerlo es necesario modificar la tabla y trabajar sobre el primal asociado</t>
+  </si>
+  <si>
+    <t>Verificamos si la solución optima lo sigue siendo (analizando el renglón $\zero$).   Caso contrario re iteramos.</t>
+  </si>
+  <si>
+    <t>Recalculamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.  Verificamos si la solución optima lo sigue siendo (analizando el renglón $\zero$) y en caso contrario re iteramos.</t>
+  </si>
+  <si>
+    <t>Recalculamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.   Verificamos si la solución optima lo sigue siendo (analizando el renglón $\zero$) y en caso contrario re iteramos.</t>
+  </si>
+  <si>
+    <t>La nueva actividad se convierte en una nueva restricción.   La re optimización es análoga al caso de nueva  restricción en el primal</t>
+  </si>
+  <si>
+    <t>La nueva restricción se convierte en una nueva actividad.    La re optimización es análoga al caso de nueva  actividad  en el primal</t>
+  </si>
+  <si>
+    <t>Tabla02.tex</t>
+  </si>
+  <si>
+    <t>Cambios en los parámetros</t>
+  </si>
+  <si>
+    <t>Propiedad de la solución afectada</t>
+  </si>
+  <si>
+    <t>Debemos recalcular el renglón $\zero$.   En caso de que no sea optimo, seguimos iterando</t>
+  </si>
+  <si>
+    <t>Verificamos si la solución optima cumple con la restricción modificada.  En caso de que no sea así modificamos la tabla y trabajamos sobre el problema dual</t>
+  </si>
+  <si>
+    <t>Agregamos una nueva columna a la tabla optima.  Verificamos si la solución optima lo sigue siendo (analizando el renglón $\zero$) y en caso contrario re iteramos.</t>
+  </si>
+  <si>
+    <t>Agregado de una nueva restricción</t>
+  </si>
+  <si>
+    <t>Verificamos si la solución optima cumple con la restricción modificada.   En caso de que no sea así modificamos la tabla y trabajamos sobre el problema dual</t>
   </si>
 </sst>
 </file>
@@ -377,29 +380,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -717,70 +720,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:J3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F5" activeCellId="1" sqref="J8 F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="20.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="30.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="2:12" s="3" customFormat="1" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="16" t="s">
+    <row r="2" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="2:12" s="3" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="E3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>3</v>
-      </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="16" t="str">
+      <c r="G3" s="11" t="str">
         <f>B3</f>
-        <v>Cambios en los parametros</v>
-      </c>
-      <c r="H3" s="16" t="str">
-        <f t="shared" ref="H3:L3" si="0">C3</f>
-        <v>Propiedad de la solucion afectada</v>
-      </c>
-      <c r="I3" s="16" t="str">
+        <v>Cambios en los parámetros</v>
+      </c>
+      <c r="H3" s="11" t="str">
+        <f t="shared" ref="H3:J3" si="0">C3</f>
+        <v>Propiedad de la solución afectada</v>
+      </c>
+      <c r="I3" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Procedimiento para reoptimizar desde el primal</v>
       </c>
-      <c r="J3" s="16" t="str">
+      <c r="J3" s="11" t="str">
         <f t="shared" si="0"/>
         <v>Procedimiento para reoptimizar desde el dual</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="2:12" s="3" customFormat="1" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" s="3" customFormat="1" ht="73" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="5" t="str">
@@ -793,56 +796,56 @@
       </c>
       <c r="I4" s="5" t="str">
         <f>CONCATENATE($E$2,D4,$F$2)</f>
-        <v>Debemos recalcular el renglon $\zero$.   En caso de que no sea optimo, seguimos iterando</v>
+        <v>Debemos recalcular el renglón $\zero$.   En caso de que no sea optimo, seguimos iterando</v>
       </c>
       <c r="J4" s="5" t="str">
         <f>CONCATENATE($E$2,E4,$F$2)</f>
-        <v>Verificamos si la solucion optima actual verifica la restriccion modificada.  En caso de no hacerlo es necesario modificar la tabla y trabajar sobre el primal asociado</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="17" t="s">
+        <v>Verificamos si la solución optima actual verifica la restricción modificada.  En caso de no hacerlo es necesario modificar la tabla y trabajar sobre el primal asociado</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>63</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="17" t="str">
+      <c r="G5" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Cambio en $b_i$</v>
       </c>
-      <c r="H5" s="17" t="str">
+      <c r="H5" s="12" t="str">
         <f t="shared" si="2"/>
         <v>Factibilidad</v>
       </c>
-      <c r="I5" s="17" t="str">
+      <c r="I5" s="12" t="str">
         <f t="shared" ref="I5:I9" si="3">CONCATENATE($E$2,D5,$F$2)</f>
-        <v>Verificamos si la solucion optima cumple con la restriccion modificada.  En caso de que no sea asi modificamos la tabla y trabajamos sobre el problema dual</v>
-      </c>
-      <c r="J5" s="17" t="str">
+        <v>Verificamos si la solución optima cumple con la restricción modificada.  En caso de que no sea así modificamos la tabla y trabajamos sobre el problema dual</v>
+      </c>
+      <c r="J5" s="12" t="str">
         <f t="shared" ref="J5:J9" si="4">CONCATENATE($E$2,E5,$F$2)</f>
-        <v>Verificamos si la solucion optima lo sigue siendo (analizando el renglon $\zero$).   Caso contrario re iteramos.</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+        <v>Verificamos si la solución optima lo sigue siendo (analizando el renglón $\zero$).   Caso contrario re iteramos.</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="3" customFormat="1" ht="87" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="5" t="str">
@@ -855,84 +858,84 @@
       </c>
       <c r="I6" s="5" t="str">
         <f t="shared" si="3"/>
-        <v>Recalulamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.  Verificamos si la solucion optima lo sigue siendo (analizando el renglon $\zero$) y en caso contrario re iteramos.</v>
+        <v>Recalculamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.  Verificamos si la solución optima lo sigue siendo (analizando el renglón $\zero$) y en caso contrario re iteramos.</v>
       </c>
       <c r="J6" s="5" t="str">
         <f t="shared" si="4"/>
-        <v>Recalulamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.  Verificamos si la solucion optima lo sigue siendo (analizando el renglon $\zero$) y en caso contrario re iteramos.</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>71</v>
+        <v>Recalculamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.  Verificamos si la solución optima lo sigue siendo (analizando el renglón $\zero$) y en caso contrario re iteramos.</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="3" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="B7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="17" t="str">
+      <c r="G7" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Cambio en $a_{ij}$ basica</v>
       </c>
-      <c r="H7" s="17" t="str">
+      <c r="H7" s="12" t="str">
         <f t="shared" si="2"/>
         <v>Factibilidad</v>
       </c>
-      <c r="I7" s="17" t="str">
+      <c r="I7" s="12" t="str">
         <f t="shared" si="3"/>
         <v>Debemos trabajar sobre el problema dual asociado</v>
       </c>
-      <c r="J7" s="17" t="str">
+      <c r="J7" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>Recalulamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.   Verificamos si la solucion optima lo sigue siendo (analizando el renglon $\zero$) y en caso contrario re iteramos.</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>65</v>
+        <v>Recalculamos la columna $A_j$ correspondiente a la $a_{ij}$ que se modifico.   Verificamos si la solución optima lo sigue siendo (analizando el renglón $\zero$) y en caso contrario re iteramos.</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" s="3" customFormat="1" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B8" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="17" t="str">
+      <c r="G8" s="12" t="str">
         <f t="shared" si="1"/>
         <v>Agregado de una nueva Actividad</v>
       </c>
-      <c r="H8" s="17" t="str">
+      <c r="H8" s="12" t="str">
         <f t="shared" si="2"/>
         <v>Optimalidad</v>
       </c>
-      <c r="I8" s="17" t="str">
+      <c r="I8" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>Agregamos una nueva columna a la tabla optima.  Verificamos si la solucion optima lo sigue siendo (analizando el renglon $\zero$) y en caso contrario re iteramos.</v>
-      </c>
-      <c r="J8" s="17" t="str">
+        <v>Agregamos una nueva columna a la tabla optima.  Verificamos si la solución optima lo sigue siendo (analizando el renglón $\zero$) y en caso contrario re iteramos.</v>
+      </c>
+      <c r="J8" s="12" t="str">
         <f t="shared" si="4"/>
-        <v>La nueva actividad se convierte en una nueva restrccion.   La reoptimizacion es analoga al caso de nueva nueva restriccion en el primal</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" s="3" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>La nueva actividad se convierte en una nueva restricción.   La re optimización es análoga al caso de nueva  restricción en el primal</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" s="3" customFormat="1" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="8" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>67</v>
@@ -940,7 +943,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="8" t="str">
         <f t="shared" si="1"/>
-        <v>Agregado de una nueva restriccion</v>
+        <v>Agregado de una nueva restricción</v>
       </c>
       <c r="H9" s="8" t="str">
         <f t="shared" si="2"/>
@@ -948,14 +951,14 @@
       </c>
       <c r="I9" s="8" t="str">
         <f t="shared" si="3"/>
-        <v>Verificamos si la solucion optima cumple con la restriccion modificada.   En caso de que no sea asi modificamos la tabla y trabajamos sobre el problema dual</v>
+        <v>Verificamos si la solución optima cumple con la restricción modificada.   En caso de que no sea así modificamos la tabla y trabajamos sobre el problema dual</v>
       </c>
       <c r="J9" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>La nueva restriccion se convierte en una nueva actividad.    La reoptimizacion es analoga al caso de nueva nueva actividad  en el primal</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>La nueva restricción se convierte en una nueva actividad.    La re optimización es análoga al caso de nueva  actividad  en el primal</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -964,45 +967,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
+        <f>COUNT(Tabla1!$G$3:$J$9)</f>
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
         <f>COUNT(Tabla2!$B$17:$J$27)</f>
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>55</v>
+      <c r="E3" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1014,288 +1035,288 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="14.7109375" style="1" customWidth="1"/>
-    <col min="3" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="9" width="16.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="14.7265625" style="1" customWidth="1"/>
+    <col min="3" max="5" width="15.7265625" style="1" customWidth="1"/>
+    <col min="6" max="9" width="16.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="18"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="2:11" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="2:11" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="I6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="J6" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="J8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="J8" s="11" t="s">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+    <row r="10" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="9"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="10" t="s">
+      <c r="H13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="2:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="4" t="s">
+      <c r="I13" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="2:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1307,64 +1328,64 @@
       <c r="J15" s="4"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="2:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="17" spans="2:10" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="J17" s="15"/>
-    </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>61</v>
       </c>
       <c r="E19" s="7" t="str">
         <f>CONCATENATE("$",E6,"$")</f>
@@ -1382,19 +1403,19 @@
         <f t="shared" si="0"/>
         <v>$y_1=2$</v>
       </c>
-      <c r="I19" s="15" t="str">
+      <c r="I19" s="18" t="str">
         <f t="shared" si="0"/>
         <v>$x_1 , x_3$</v>
       </c>
-      <c r="J19" s="15" t="str">
+      <c r="J19" s="18" t="str">
         <f t="shared" si="0"/>
         <v>$y_2 , y_4$</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+    <row r="20" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="9" t="str">
         <f>CONCATENATE("$",E7,"$")</f>
         <v>$x_2 \rightarrow y_4$</v>
@@ -1411,18 +1432,18 @@
         <f t="shared" si="0"/>
         <v>$y_3=0$</v>
       </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>13</v>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+    </row>
+    <row r="21" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="E21" s="10" t="str">
         <f>CONCATENATE("$",E8,"$")</f>
@@ -1440,19 +1461,19 @@
         <f t="shared" si="0"/>
         <v>$y_2=5.6$</v>
       </c>
-      <c r="I21" s="11" t="str">
+      <c r="I21" s="14" t="str">
         <f t="shared" si="0"/>
         <v>$x_4, x_5$</v>
       </c>
-      <c r="J21" s="11" t="str">
+      <c r="J21" s="14" t="str">
         <f t="shared" si="0"/>
         <v>$y_1, y_5, y_4$</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
+    <row r="22" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
       <c r="E22" s="4" t="str">
         <f>CONCATENATE("$",E9,"$")</f>
         <v>$x_2 \rightarrow y_5$</v>
@@ -1469,13 +1490,13 @@
         <f t="shared" si="0"/>
         <v>$y_3=5.3$</v>
       </c>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9" t="str">
         <f t="shared" si="0"/>
@@ -1486,18 +1507,18 @@
         <v>$x_2=2$</v>
       </c>
       <c r="H23" s="9"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="11" t="s">
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>10</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="E24" s="10" t="str">
         <f>CONCATENATE("$",E11,"$")</f>
@@ -1515,19 +1536,19 @@
         <f t="shared" si="0"/>
         <v>$y_2=1$</v>
       </c>
-      <c r="I24" s="11" t="str">
+      <c r="I24" s="14" t="str">
         <f t="shared" si="0"/>
         <v>$x_3, x_4$</v>
       </c>
-      <c r="J24" s="11" t="str">
+      <c r="J24" s="14" t="str">
         <f t="shared" si="0"/>
         <v>$y_1, y_3, y_4$</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
+    <row r="25" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
       <c r="E25" s="9" t="str">
         <f>CONCATENATE("$",E12,"$")</f>
         <v>$x_2 \rightarrow y_4$</v>
@@ -1544,18 +1565,18 @@
         <f t="shared" si="0"/>
         <v>$ \mu_2=1$</v>
       </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>14</v>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="E26" s="4" t="str">
         <f>CONCATENATE("$",E13,"$")</f>
@@ -1573,19 +1594,19 @@
         <f t="shared" si="0"/>
         <v>$y_2=4.5$</v>
       </c>
-      <c r="I26" s="11" t="str">
+      <c r="I26" s="14" t="str">
         <f t="shared" si="0"/>
         <v>$x_1, x_3 , x_4$</v>
       </c>
-      <c r="J26" s="11" t="str">
+      <c r="J26" s="14" t="str">
         <f t="shared" si="0"/>
         <v>$y_1, y_4$</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
+    <row r="27" spans="2:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
       <c r="E27" s="6" t="str">
         <f>CONCATENATE("$",E14,"$")</f>
         <v>$x_2 \rightarrow y_4$</v>
@@ -1602,44 +1623,18 @@
         <f t="shared" si="0"/>
         <v>$y_3=1.5$</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-    </row>
-    <row r="28" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
@@ -1650,12 +1645,38 @@
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="I19:I20"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="I21:I23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>